<commit_message>
Removed - ToborAutomator-EmailHandler Added - ToborInc-Email
ToboInc-Emails Supports
	Checking Subject, Checking Conent, Registering User.
</commit_message>
<xml_diff>
--- a/Project (UiPath)/ToborInc-Files/Database.xlsx
+++ b/Project (UiPath)/ToborInc-Files/Database.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\QA Workspace\SFIA Project 2\Project (UiPath)\ToborInc-Files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EA75BB27-B7BA-4B83-9738-D82CB418442D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{434C2C90-39BF-41FF-91AE-23BCD5ECBC70}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="5280" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="10935" yWindow="390" windowWidth="17700" windowHeight="15435" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Customer_Database" sheetId="2" r:id="rId1"/>
@@ -1271,10 +1271,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{47725217-C61D-4A6A-B15B-CE010EB9806A}">
-  <dimension ref="A1:I51"/>
+  <dimension ref="A1:I56"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
+      <selection activeCell="D57" sqref="D57"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2767,6 +2767,21 @@
         <v>44005</v>
       </c>
     </row>
+    <row r="52" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="I52" s="1"/>
+    </row>
+    <row r="53" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="I53" s="1"/>
+    </row>
+    <row r="54" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="I54" s="1"/>
+    </row>
+    <row r="55" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="I55" s="1"/>
+    </row>
+    <row r="56" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="I56" s="1"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>